<commit_message>
Added Two more leet problems
</commit_message>
<xml_diff>
--- a/MySQL/Exhaustive List.xlsx
+++ b/MySQL/Exhaustive List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="129">
   <si>
     <t>Topic</t>
   </si>
@@ -787,12 +787,35 @@
 WHERE (id+2)%2=1 AND description &lt;&gt; 'boring'
 ORDER BY rating DESC;</t>
   </si>
+  <si>
+    <t>https://leetcode.com/problems/duplicate-emails/description/</t>
+  </si>
+  <si>
+    <t>Suggested Solution:
+SELECT Email
+FROM Person
+GROUP BY Email
+HAVING COUNT(Email) &gt; 1;</t>
+  </si>
+  <si>
+    <t>Hard Way :)
+SELECT DISTINCT(p1.Email) from Person p1,  Person p2
+WHERE p1.Email = p2.Email AND p1.Id&lt;&gt;p2.Id;</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combine-two-tables/description/</t>
+  </si>
+  <si>
+    <t>SELECT FirstName, LastName, City, State
+FROM Person LEFT JOIN Address
+ON Person.PersonId = Address.PersonId;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -849,16 +872,35 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="15"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -894,7 +936,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -950,17 +992,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1267,7 +1312,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>527049</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>164596</xdr:rowOff>
+      <xdr:rowOff>62996</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1311,7 +1356,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>241114</xdr:rowOff>
+      <xdr:rowOff>126814</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1336,6 +1381,94 @@
         <a:xfrm>
           <a:off x="609600" y="6254750"/>
           <a:ext cx="8458200" cy="4584514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542011</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34C45630-8679-4AC2-B5B6-0712FD6F0749}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="673100" y="11372851"/>
+          <a:ext cx="8219161" cy="3225800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>655</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A54ACD-C752-4A29-81AA-491637357720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16478250"/>
+          <a:ext cx="8350905" cy="5226050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1612,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3081,24 +3214,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE1F944-BB59-4556-A64F-E6C0CCFD897C}">
   <dimension ref="A1:R244"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="16"/>
-    <col min="2" max="2" width="49.7265625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="21"/>
+    <col min="2" max="2" width="49.7265625" style="23" customWidth="1"/>
     <col min="3" max="11" width="8.7265625" style="16"/>
     <col min="12" max="12" width="22.453125" style="16" customWidth="1"/>
     <col min="13" max="13" width="8.7265625" style="16"/>
-    <col min="14" max="14" width="64.7265625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="66.7265625" style="20" customWidth="1"/>
     <col min="15" max="15" width="8.7265625" style="16"/>
     <col min="17" max="17" width="8.7265625" style="16"/>
     <col min="19" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="17" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -3108,1237 +3241,1258 @@
       <c r="L1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="21"/>
-    </row>
-    <row r="2" spans="1:14" ht="57" x14ac:dyDescent="0.4">
-      <c r="A2" s="16">
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="1:14" ht="58.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>121</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="20" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L3" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L4" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L5" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L6" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L7" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L8" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L9" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L10" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L11" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L12" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L13" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L14" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L15" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L16" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L17" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L18" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L19" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="57" x14ac:dyDescent="0.4">
-      <c r="A20" s="16">
+    <row r="20" spans="1:14" ht="58.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="21">
         <v>2</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="22" t="s">
         <v>122</v>
       </c>
       <c r="L20" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="N20" s="22" t="s">
+      <c r="N20" s="20" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L21" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L22" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L23" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L24" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L25" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L26" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L27" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L28" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L29" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L30" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L31" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L32" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L33" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L34" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L35" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L36" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L37" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L38" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L39" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L40" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L41" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" ht="78" x14ac:dyDescent="0.45">
+      <c r="A42" s="21">
+        <v>3</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>124</v>
+      </c>
       <c r="L42" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="N42" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L43" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" ht="117" x14ac:dyDescent="0.45">
       <c r="L44" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="45" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="N44" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L45" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L46" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L47" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L48" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L49" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L50" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L51" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L52" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:14" ht="58.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="21">
+        <v>4</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>127</v>
+      </c>
       <c r="L53" s="16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="54" spans="12:12" x14ac:dyDescent="0.4">
+      <c r="N53" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L54" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L55" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L56" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L57" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L58" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L59" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L60" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L61" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L62" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L63" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L64" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="65" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L65" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="66" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L66" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="67" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L67" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="68" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L68" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="69" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L69" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="70" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L70" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="71" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="71" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L71" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="72" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L72" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="73" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L73" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="74" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="74" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L74" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="75" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L75" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="76" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L76" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="77" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L77" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="78" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="78" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L78" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="79" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L79" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="80" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L80" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="81" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L81" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="82" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="82" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L82" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="83" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L83" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="84" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="84" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L84" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="85" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="85" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L85" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="86" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L86" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="87" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L87" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="88" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L88" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="89" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L89" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="90" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L90" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="91" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L91" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="92" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="92" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L92" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="93" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L93" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="94" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L94" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="95" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L95" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="96" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L96" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="97" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L97" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="98" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L98" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="99" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="99" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L99" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="100" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="100" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L100" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="101" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L101" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="102" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="102" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L102" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="103" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="103" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L103" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="104" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="104" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L104" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="105" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L105" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="106" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L106" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="107" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L107" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="108" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="108" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L108" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="109" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L109" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="110" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L110" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="111" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="111" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L111" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="112" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L112" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="113" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="113" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L113" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="114" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L114" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="115" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L115" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="116" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L116" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="117" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="117" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L117" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="118" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="118" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L118" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="119" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="119" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L119" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="120" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L120" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="121" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L121" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="122" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L122" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="123" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L123" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="124" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L124" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="125" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="125" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L125" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="126" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="126" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L126" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="127" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L127" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="128" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L128" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="129" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L129" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="130" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="130" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L130" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="131" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="131" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L131" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="132" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="132" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L132" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="133" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="133" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L133" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="134" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="134" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L134" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="135" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="135" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L135" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="136" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="136" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L136" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="137" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L137" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="138" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="138" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L138" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="139" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="139" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L139" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="140" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L140" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="141" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="141" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L141" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="142" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="142" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L142" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="143" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="143" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L143" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="144" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="144" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L144" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="145" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="145" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L145" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="146" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="146" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L146" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="147" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="147" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L147" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="148" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="148" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L148" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="149" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="149" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L149" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="150" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="150" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L150" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="151" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="151" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L151" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="152" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="152" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L152" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="153" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="153" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L153" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="154" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="154" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L154" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="155" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="155" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L155" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="156" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L156" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="157" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="157" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L157" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="158" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="158" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L158" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="159" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="159" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L159" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="160" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="160" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L160" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="161" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="161" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L161" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="162" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="162" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L162" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="163" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="163" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L163" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="164" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="164" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L164" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="165" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="165" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L165" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="166" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="166" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L166" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="167" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="167" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L167" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="168" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="168" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L168" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="169" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="169" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L169" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="170" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="170" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L170" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="171" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="171" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L171" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="172" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="172" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L172" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="173" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="173" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L173" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="174" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="174" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L174" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="175" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="175" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L175" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="176" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="176" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L176" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="177" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="177" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L177" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="178" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="178" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L178" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="179" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="179" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L179" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="180" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="180" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L180" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="181" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="181" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L181" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="182" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="182" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L182" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="183" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="183" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L183" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="184" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="184" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L184" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="185" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="185" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L185" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="186" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="186" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L186" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="187" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="187" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L187" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="188" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="188" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L188" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="189" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="189" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L189" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="190" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L190" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="191" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="191" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L191" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="192" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="192" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L192" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="193" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="193" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L193" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="194" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="194" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L194" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="195" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="195" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L195" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="196" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="196" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L196" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="197" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="197" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L197" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="198" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="198" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L198" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="199" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="199" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L199" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="200" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="200" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L200" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="201" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="201" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L201" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="202" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="202" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L202" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="203" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="203" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L203" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="204" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="204" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L204" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="205" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="205" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L205" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="206" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="206" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L206" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="207" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="207" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L207" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="208" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="208" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L208" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="209" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="209" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L209" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="210" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="210" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L210" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="211" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="211" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L211" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="212" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="212" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L212" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="213" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="213" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L213" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="214" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="214" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L214" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="215" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="215" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L215" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="216" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="216" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L216" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="217" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="217" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L217" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="218" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="218" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L218" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="219" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="219" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L219" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="220" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="220" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L220" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="221" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="221" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L221" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="222" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="222" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L222" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="223" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="223" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L223" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="224" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="224" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L224" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="225" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="225" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L225" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="226" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="226" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L226" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="227" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="227" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L227" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="228" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="228" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L228" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="229" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="229" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L229" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="230" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="230" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L230" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="231" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="231" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L231" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="232" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="232" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L232" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="233" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="233" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L233" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="234" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="234" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L234" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="235" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="235" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L235" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="236" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="236" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L236" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="237" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="237" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L237" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="238" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="238" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L238" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="239" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="239" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L239" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="240" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="240" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L240" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="241" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="241" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L241" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="242" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="242" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L242" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="243" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="243" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L243" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="244" spans="12:12" x14ac:dyDescent="0.4">
+    <row r="244" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L244" s="16" t="s">
         <v>119</v>
       </c>
@@ -4346,9 +4500,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F578D9F1-7A3F-4F24-B69C-5145A8CC103A}"/>
+    <hyperlink ref="B42" r:id="rId2" xr:uid="{DBB76FA3-C7F6-4B58-966D-87BD06426FDD}"/>
+    <hyperlink ref="B53" r:id="rId3" xr:uid="{53475170-E1EB-47DF-BCC7-B412EBB817DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>